<commit_message>
Aggiornate immagini normalizzazione, aggiunto schema relazionale
</commit_message>
<xml_diff>
--- a/Relazione/normalizzazione.xlsx
+++ b/Relazione/normalizzazione.xlsx
@@ -107,9 +107,6 @@
     <t>PERMESSI_UTENTE</t>
   </si>
   <si>
-    <t>idRuolo</t>
-  </si>
-  <si>
     <t>idUtente</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>numeroCivico</t>
+  </si>
+  <si>
+    <t>idPermesso</t>
   </si>
 </sst>
 </file>
@@ -352,18 +352,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,11 +362,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -390,16 +390,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6878,145 +6878,145 @@
   </sheetPr>
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="11"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:14" s="8" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
+      <c r="I8" s="13"/>
+      <c r="J8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
@@ -7027,68 +7027,68 @@
         <v>9</v>
       </c>
       <c r="E12" s="16"/>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
@@ -7099,338 +7099,338 @@
         <v>8</v>
       </c>
       <c r="E20" s="16"/>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
+      <c r="G20" s="13"/>
+      <c r="H20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="5"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="2:14" s="8" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+    <row r="24" spans="2:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="17"/>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4" t="s">
+      <c r="F24" s="13"/>
+      <c r="G24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
+      <c r="J24" s="13"/>
+      <c r="K24" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3" t="s">
+      <c r="L24" s="13"/>
+      <c r="M24" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N24" s="5"/>
+      <c r="N24" s="14"/>
     </row>
     <row r="25" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="2:14" s="9" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+    <row r="28" spans="2:14" s="5" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="4" t="s">
+      <c r="E28" s="19"/>
+      <c r="F28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3" t="s">
+      <c r="I28" s="13"/>
+      <c r="J28" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="5"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="2:14" s="8" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+    <row r="32" spans="2:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3" t="s">
+      <c r="E32" s="13"/>
+      <c r="F32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3" t="s">
+      <c r="G32" s="13"/>
+      <c r="H32" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3" t="s">
+      <c r="I32" s="13"/>
+      <c r="J32" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="5"/>
+      <c r="K32" s="14"/>
     </row>
     <row r="33" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
     </row>
     <row r="36" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3" t="s">
+      <c r="E36" s="13"/>
+      <c r="F36" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
+      <c r="G36" s="13"/>
+      <c r="H36" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="5"/>
+      <c r="I36" s="14"/>
     </row>
     <row r="37" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
     </row>
     <row r="40" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F40" s="17"/>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3" t="s">
+      <c r="H40" s="13"/>
+      <c r="I40" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J40" s="5"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
+      <c r="B43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
     </row>
-    <row r="44" spans="2:13" s="8" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+    <row r="44" spans="2:13" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="17"/>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3" t="s">
+      <c r="F44" s="13"/>
+      <c r="G44" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J44" s="3" t="s">
+      <c r="H44" s="13"/>
+      <c r="I44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3" t="s">
+      <c r="K44" s="13"/>
+      <c r="L44" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="5"/>
+      <c r="M44" s="14"/>
     </row>
     <row r="45" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
+      <c r="B47" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
     </row>
     <row r="48" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="17"/>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3" t="s">
+      <c r="F48" s="13"/>
+      <c r="G48" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3" t="s">
+      <c r="J48" s="13"/>
+      <c r="K48" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L48" s="5"/>
+      <c r="L48" s="14"/>
     </row>
     <row r="49" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
+      <c r="B51" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
     </row>
     <row r="52" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E52" s="16"/>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3" t="s">
+      <c r="G52" s="13"/>
+      <c r="H52" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="5"/>
+      <c r="I52" s="14"/>
     </row>
     <row r="53" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
     </row>
     <row r="55" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7497,6 +7497,16 @@
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="H52:I52"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="L44:M44"/>
     <mergeCell ref="B47:K47"/>
@@ -7513,16 +7523,6 @@
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="G44:H44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="B27:K27"/>
     <mergeCell ref="B31:K31"/>
@@ -7542,17 +7542,17 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Modificate alcune cose sulla relazione e caricate nuove immagini
Vanno corrette le immagini (e tutto quello che ti ho detto su Telegram)
</commit_message>
<xml_diff>
--- a/Relazione/normalizzazione.xlsx
+++ b/Relazione/normalizzazione.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="880" windowWidth="36480" windowHeight="22880" xr2:uid="{BDFE7E85-4550-374A-B61E-33AFACDC1E5D}"/>
+    <workbookView xWindow="1920" yWindow="440" windowWidth="36480" windowHeight="21160" xr2:uid="{BDFE7E85-4550-374A-B61E-33AFACDC1E5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -101,12 +101,6 @@
     <t xml:space="preserve">nome </t>
   </si>
   <si>
-    <t>PERMESSI</t>
-  </si>
-  <si>
-    <t>PERMESSI_UTENTE</t>
-  </si>
-  <si>
     <t>idUtente</t>
   </si>
   <si>
@@ -168,6 +162,12 @@
   </si>
   <si>
     <t>idPermesso</t>
+  </si>
+  <si>
+    <t>PERMESSO</t>
+  </si>
+  <si>
+    <t>PERMESSO_UTENTE</t>
   </si>
 </sst>
 </file>
@@ -369,17 +369,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,11 +399,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6879,24 +6879,24 @@
   <dimension ref="A1:N106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
@@ -6906,27 +6906,27 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="K2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="10" t="s">
+      <c r="L2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>19</v>
@@ -6936,28 +6936,28 @@
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13" t="s">
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="14"/>
@@ -6965,39 +6965,39 @@
     <row r="5" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="14"/>
@@ -7005,33 +7005,33 @@
     <row r="9" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13" t="s">
+      <c r="G12" s="11"/>
+      <c r="H12" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I12" s="14"/>
@@ -7039,18 +7039,18 @@
     <row r="13" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
@@ -7065,11 +7065,11 @@
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13" t="s">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I16" s="14"/>
@@ -7077,33 +7077,33 @@
     <row r="17" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
     </row>
     <row r="20" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="13" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I20" s="14"/>
@@ -7111,46 +7111,46 @@
     <row r="21" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="2:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="13" t="s">
+      <c r="D24" s="18"/>
+      <c r="E24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13" t="s">
+      <c r="J24" s="11"/>
+      <c r="K24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13" t="s">
+      <c r="L24" s="11"/>
+      <c r="M24" s="11" t="s">
         <v>7</v>
       </c>
       <c r="N24" s="14"/>
@@ -7158,39 +7158,39 @@
     <row r="25" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
     </row>
     <row r="28" spans="2:14" s="5" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="19"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13" t="s">
+      <c r="I28" s="11"/>
+      <c r="J28" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K28" s="14"/>
@@ -7198,18 +7198,18 @@
     <row r="29" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="2:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
     </row>
     <row r="32" spans="2:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
@@ -7218,19 +7218,19 @@
       <c r="C32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13" t="s">
+      <c r="E32" s="11"/>
+      <c r="F32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13" t="s">
+      <c r="G32" s="11"/>
+      <c r="H32" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13" t="s">
+      <c r="I32" s="11"/>
+      <c r="J32" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K32" s="14"/>
@@ -7238,18 +7238,18 @@
     <row r="33" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
+      <c r="B35" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
     </row>
     <row r="36" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
@@ -7258,15 +7258,15 @@
       <c r="C36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13" t="s">
+      <c r="E36" s="11"/>
+      <c r="F36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13" t="s">
+      <c r="G36" s="11"/>
+      <c r="H36" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I36" s="14"/>
@@ -7274,36 +7274,36 @@
     <row r="37" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
+      <c r="B39" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
     </row>
     <row r="40" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="13" t="s">
+      <c r="C40" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13" t="s">
+      <c r="H40" s="11"/>
+      <c r="I40" s="11" t="s">
         <v>7</v>
       </c>
       <c r="J40" s="14"/>
@@ -7311,43 +7311,43 @@
     <row r="41" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
+      <c r="B43" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
     </row>
     <row r="44" spans="2:13" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="13" t="s">
+      <c r="D44" s="18"/>
+      <c r="E44" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13" t="s">
+      <c r="F44" s="11"/>
+      <c r="G44" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H44" s="13"/>
+      <c r="H44" s="11"/>
       <c r="I44" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J44" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13" t="s">
+      <c r="K44" s="11"/>
+      <c r="L44" s="11" t="s">
         <v>7</v>
       </c>
       <c r="M44" s="14"/>
@@ -7355,40 +7355,40 @@
     <row r="45" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
+      <c r="B47" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
     </row>
     <row r="48" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="13" t="s">
+      <c r="D48" s="18"/>
+      <c r="E48" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13" t="s">
+      <c r="F48" s="11"/>
+      <c r="G48" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13" t="s">
+      <c r="J48" s="11"/>
+      <c r="K48" s="11" t="s">
         <v>7</v>
       </c>
       <c r="L48" s="14"/>
@@ -7396,33 +7396,33 @@
     <row r="49" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
+      <c r="B51" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
     </row>
     <row r="52" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16" t="s">
+      <c r="B52" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="13" t="s">
+      <c r="E52" s="17"/>
+      <c r="F52" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13" t="s">
+      <c r="G52" s="11"/>
+      <c r="H52" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I52" s="14"/>
@@ -7486,11 +7486,52 @@
     <row r="106" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B23:K23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="B51:K51"/>
     <mergeCell ref="B52:C52"/>
@@ -7507,52 +7548,11 @@
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Corrette di nuovo le immagini e aggiornata relazione
</commit_message>
<xml_diff>
--- a/Relazione/normalizzazione.xlsx
+++ b/Relazione/normalizzazione.xlsx
@@ -383,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -417,40 +417,37 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -462,8 +459,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6941,25 +6947,25 @@
   </sheetPr>
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="177" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:P24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="177" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
@@ -6971,17 +6977,17 @@
       <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="20"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="10" t="s">
         <v>37</v>
       </c>
@@ -6999,10 +7005,10 @@
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
@@ -7012,108 +7018,108 @@
       <c r="F4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19" t="s">
+      <c r="H4" s="17"/>
+      <c r="I4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19" t="s">
+      <c r="J4" s="17"/>
+      <c r="K4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="21"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="21"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="19" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19" t="s">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="21"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
@@ -7128,155 +7134,155 @@
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="21"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
     </row>
     <row r="20" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="19" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="21"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
     </row>
     <row r="24" spans="2:16" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15" t="s">
+      <c r="D24" s="21"/>
+      <c r="E24" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="17" t="s">
+      <c r="F24" s="22"/>
+      <c r="G24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
       <c r="I24" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K24" s="16" t="s">
+      <c r="K24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="17"/>
-      <c r="M24" s="16" t="s">
+      <c r="L24" s="23"/>
+      <c r="M24" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N24" s="17"/>
-      <c r="O24" s="16" t="s">
+      <c r="N24" s="23"/>
+      <c r="O24" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="P24" s="18"/>
+      <c r="P24" s="14"/>
     </row>
     <row r="25" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
     </row>
     <row r="28" spans="2:16" s="5" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27" t="s">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="27"/>
+      <c r="E28" s="26"/>
       <c r="F28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19" t="s">
+      <c r="I28" s="17"/>
+      <c r="J28" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="21"/>
+      <c r="K28" s="18"/>
     </row>
     <row r="29" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
     </row>
     <row r="32" spans="2:16" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
@@ -7285,38 +7291,38 @@
       <c r="C32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19" t="s">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19" t="s">
+      <c r="G32" s="17"/>
+      <c r="H32" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19" t="s">
+      <c r="I32" s="17"/>
+      <c r="J32" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="21"/>
+      <c r="K32" s="18"/>
     </row>
     <row r="33" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
     </row>
     <row r="36" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
@@ -7325,171 +7331,171 @@
       <c r="C36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19" t="s">
+      <c r="E36" s="17"/>
+      <c r="F36" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19" t="s">
+      <c r="G36" s="17"/>
+      <c r="H36" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="21"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
     </row>
     <row r="40" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="15" t="s">
+      <c r="C40" s="29"/>
+      <c r="D40" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="16" t="s">
+      <c r="E40" s="29"/>
+      <c r="F40" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="16" t="s">
+      <c r="G40" s="23"/>
+      <c r="H40" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I40" s="18"/>
+      <c r="I40" s="14"/>
     </row>
     <row r="41" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
     </row>
     <row r="44" spans="2:13" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="19" t="s">
+      <c r="D44" s="24"/>
+      <c r="E44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19" t="s">
+      <c r="F44" s="17"/>
+      <c r="G44" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H44" s="19"/>
+      <c r="H44" s="17"/>
       <c r="I44" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J44" s="19" t="s">
+      <c r="J44" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19" t="s">
+      <c r="K44" s="17"/>
+      <c r="L44" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="21"/>
+      <c r="M44" s="18"/>
     </row>
     <row r="45" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="22"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
     </row>
     <row r="48" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="19" t="s">
+      <c r="D48" s="24"/>
+      <c r="E48" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19" t="s">
+      <c r="F48" s="17"/>
+      <c r="G48" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19" t="s">
+      <c r="H48" s="17"/>
+      <c r="I48" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19" t="s">
+      <c r="J48" s="17"/>
+      <c r="K48" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L48" s="21"/>
+      <c r="L48" s="18"/>
     </row>
     <row r="49" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
     </row>
     <row r="52" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24" t="s">
+      <c r="C52" s="20"/>
+      <c r="D52" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="19" t="s">
+      <c r="E52" s="20"/>
+      <c r="F52" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19" t="s">
+      <c r="G52" s="17"/>
+      <c r="H52" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="21"/>
+      <c r="I52" s="18"/>
     </row>
     <row r="53" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -7550,6 +7556,58 @@
     <row r="106" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B23:K23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B15:K15"/>
@@ -7566,58 +7624,6 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="B19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Corretta relazione e immagini
</commit_message>
<xml_diff>
--- a/Relazione/normalizzazione.xlsx
+++ b/Relazione/normalizzazione.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1920" windowWidth="36480" windowHeight="21160" xr2:uid="{BDFE7E85-4550-374A-B61E-33AFACDC1E5D}"/>
+    <workbookView xWindow="1420" yWindow="1000" windowWidth="36480" windowHeight="21160" xr2:uid="{BDFE7E85-4550-374A-B61E-33AFACDC1E5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -417,22 +417,43 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,34 +462,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3634,62 +3634,6 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="6611057" y="10944224"/>
-          <a:ext cx="0" cy="250825"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>16581</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>349248</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>16581</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>234948</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="92" name="Connettore 2 91">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF8A60CD-91AC-5A48-A0DE-C069B57E9F0E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4144081" y="12398373"/>
           <a:ext cx="0" cy="250825"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -6623,6 +6567,61 @@
             <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>34146</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9172</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>34146</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>237816</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="114" name="Connettore 1 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B489C602-A1E5-8B43-B579-738E7A721342}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3334711" y="14646460"/>
+          <a:ext cx="0" cy="228644"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -6948,24 +6947,24 @@
   <dimension ref="A1:P106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="177" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
@@ -6977,17 +6976,17 @@
       <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="27"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="10" t="s">
         <v>37</v>
       </c>
@@ -7005,10 +7004,10 @@
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
@@ -7018,108 +7017,108 @@
       <c r="F4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17" t="s">
+      <c r="J4" s="19"/>
+      <c r="K4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="18"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17" t="s">
+      <c r="G8" s="19"/>
+      <c r="H8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="18"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="17" t="s">
+      <c r="E12" s="27"/>
+      <c r="F12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17" t="s">
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="18"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
@@ -7134,64 +7133,64 @@
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17" t="s">
+      <c r="G16" s="19"/>
+      <c r="H16" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="18"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
     </row>
     <row r="20" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20" t="s">
+      <c r="C20" s="27"/>
+      <c r="D20" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="27"/>
+      <c r="F20" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17" t="s">
+      <c r="G20" s="19"/>
+      <c r="H20" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="18"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
     </row>
     <row r="24" spans="2:16" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
@@ -7200,89 +7199,89 @@
       <c r="C24" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23" t="s">
+      <c r="F24" s="30"/>
+      <c r="G24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="23"/>
-      <c r="M24" s="13" t="s">
+      <c r="L24" s="17"/>
+      <c r="M24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="N24" s="23"/>
-      <c r="O24" s="13" t="s">
+      <c r="N24" s="17"/>
+      <c r="O24" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P24" s="14"/>
+      <c r="P24" s="18"/>
     </row>
     <row r="25" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
     </row>
     <row r="28" spans="2:16" s="5" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26" t="s">
+      <c r="C28" s="22"/>
+      <c r="D28" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="26"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17" t="s">
+      <c r="I28" s="19"/>
+      <c r="J28" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="21"/>
     </row>
     <row r="29" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="2:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
     </row>
     <row r="32" spans="2:16" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
@@ -7291,38 +7290,38 @@
       <c r="C32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17" t="s">
+      <c r="E32" s="19"/>
+      <c r="F32" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17" t="s">
+      <c r="G32" s="19"/>
+      <c r="H32" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17" t="s">
+      <c r="I32" s="19"/>
+      <c r="J32" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="18"/>
+      <c r="K32" s="21"/>
     </row>
     <row r="33" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
     </row>
     <row r="36" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
@@ -7331,68 +7330,68 @@
       <c r="C36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17" t="s">
+      <c r="E36" s="19"/>
+      <c r="F36" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17" t="s">
+      <c r="G36" s="19"/>
+      <c r="H36" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="18"/>
+      <c r="I36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
     </row>
     <row r="40" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="13" t="s">
+      <c r="E40" s="14"/>
+      <c r="F40" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="23"/>
-      <c r="H40" s="13" t="s">
+      <c r="G40" s="17"/>
+      <c r="H40" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I40" s="14"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
     </row>
     <row r="44" spans="2:13" s="4" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
@@ -7402,41 +7401,41 @@
         <v>17</v>
       </c>
       <c r="D44" s="24"/>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17" t="s">
+      <c r="F44" s="19"/>
+      <c r="G44" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H44" s="17"/>
+      <c r="H44" s="19"/>
       <c r="I44" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J44" s="17" t="s">
+      <c r="J44" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17" t="s">
+      <c r="K44" s="19"/>
+      <c r="L44" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="18"/>
+      <c r="M44" s="21"/>
     </row>
     <row r="45" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
     </row>
     <row r="48" spans="2:13" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
@@ -7446,56 +7445,56 @@
         <v>17</v>
       </c>
       <c r="D48" s="24"/>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17" t="s">
+      <c r="F48" s="19"/>
+      <c r="G48" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17" t="s">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17" t="s">
+      <c r="J48" s="19"/>
+      <c r="K48" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="L48" s="18"/>
+      <c r="L48" s="21"/>
     </row>
     <row r="49" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
     </row>
     <row r="52" spans="2:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20" t="s">
+      <c r="C52" s="27"/>
+      <c r="D52" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="17" t="s">
+      <c r="E52" s="27"/>
+      <c r="F52" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17" t="s">
+      <c r="G52" s="19"/>
+      <c r="H52" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="18"/>
+      <c r="I52" s="21"/>
     </row>
     <row r="53" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="2:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -7556,6 +7555,58 @@
     <row r="106" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="F40:G40"/>
@@ -7572,58 +7623,6 @@
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>